<commit_message>
Fixed all projects being shown
</commit_message>
<xml_diff>
--- a/server/data/projects.xlsx
+++ b/server/data/projects.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -502,9 +502,56 @@
         <v>1744003083264</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1744625747268</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Caterpillar</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Hybrid Seat Allocation</v>
+      </c>
+      <c r="E3" t="str">
+        <v>PI</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Copi</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2023-2024</v>
+      </c>
+      <c r="H3" t="str">
+        <v>20000</v>
+      </c>
+      <c r="I3" t="str">
+        <v>10000</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Details</v>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v>h</v>
+      </c>
+      <c r="M3" t="str">
+        <v>agreementDocument-1744625747215-658333568.pdf</v>
+      </c>
+      <c r="O3" t="str">
+        <v>2025-04-14T10:15:47.268Z</v>
+      </c>
+      <c r="P3" t="str">
+        <v>1744624259342</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dark themed design updates
</commit_message>
<xml_diff>
--- a/server/data/projects.xlsx
+++ b/server/data/projects.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -549,9 +549,59 @@
         <v>1744624259342</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1744633011051</v>
+      </c>
+      <c r="B4" t="str">
+        <v>strategy fox</v>
+      </c>
+      <c r="C4" t="str">
+        <v>3</v>
+      </c>
+      <c r="D4" t="str">
+        <v>VR game</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Vishal</v>
+      </c>
+      <c r="F4" t="str">
+        <v>NA</v>
+      </c>
+      <c r="G4" t="str">
+        <v>2023-2024</v>
+      </c>
+      <c r="H4" t="str">
+        <v>50000</v>
+      </c>
+      <c r="I4" t="str">
+        <v>50000</v>
+      </c>
+      <c r="J4" t="str">
+        <v>NA</v>
+      </c>
+      <c r="K4" t="str">
+        <v>NA</v>
+      </c>
+      <c r="L4" t="str">
+        <v>NA</v>
+      </c>
+      <c r="M4" t="str">
+        <v>agreementDocument-1744633011045-909105401.pdf</v>
+      </c>
+      <c r="N4" t="str">
+        <v>billSettlementProof-1744633011043-117583223.pdf</v>
+      </c>
+      <c r="O4" t="str">
+        <v>2025-04-14T12:16:51.051Z</v>
+      </c>
+      <c r="P4" t="str">
+        <v>1744003743096</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>